<commit_message>
Improve Whole Foods order processing by standardizing item number formats
Adds item mapping to normalize Whole Foods product numbers with spaces and dashes.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a4c793ea-64cf-4601-8936-3568869ffe5a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/c5fd0f16-2d84-4af3-99b4-3191adee6a6a/a4c793ea-64cf-4601-8936-3568869ffe5a/VQxL7ot
</commit_message>
<xml_diff>
--- a/mappings/wholefoods/item_mapping.xlsx
+++ b/mappings/wholefoods/item_mapping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,72 +448,348 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>WF-ITEM-001</t>
+          <t>12-046-2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>WF-ITEM-001</t>
+          <t>12-046-2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>WF-ITEM-002</t>
+          <t>12 046 3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>WF-ITEM-002</t>
+          <t>12-046-3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>WF-ITEM-003</t>
+          <t>130251</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>WF-ITEM-003</t>
+          <t>13-025-1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ORGANIC-BANANAS-001</t>
+          <t>13 025 126</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ORGANIC-BANANAS-001</t>
+          <t>13-025-126</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ORGANIC-APPLES-002</t>
+          <t>1302514</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ORGANIC-APPLES-002</t>
+          <t>13-025-14</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>UNKNOWN</t>
+          <t>1302515</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>UNKNOWN</t>
+          <t>13-025-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1302517</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>13-025-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>130252</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>13-025-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1302520</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>13-025-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>13 025 24</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>13-025-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>13-025-25</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>13-025-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>13-025-26</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>13-025-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>130253</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>13-025-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>130254</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>13-025-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>130255</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>13-025-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>130256</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>13-025-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>130257</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>13-025-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>130258</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>13-025-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>130259</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>13-025-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>13-027-1</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>13-027-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>13-027-2</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>13-027-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>13-027-3</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>13-027-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>13-027-4</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>13-027-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>170411</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>17-041-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>170417</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>17-041-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>170512</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>17-051-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>6016</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>6-016</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>90311</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>9-031-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>90881</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>9-088-1</t>
         </is>
       </c>
     </row>

</xml_diff>